<commit_message>
changed some graphs colors and labels
</commit_message>
<xml_diff>
--- a/data/raw/incidencia.xlsx
+++ b/data/raw/incidencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipesn/Documents/R/despliegue_guardia_nacional/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0810DFCB-F226-5440-84C4-E2528A41775F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992647AE-3663-DD4E-840A-4E400D158335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35220" windowHeight="16960" xr2:uid="{92BB36FF-57BC-46A4-9CFB-F77641F9D7F4}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>Guerrero</t>
   </si>
   <si>
-    <t>Michoacan</t>
-  </si>
-  <si>
     <t>Homicidio doloso y feminicidio</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>delito</t>
+  </si>
+  <si>
+    <t>Michoacán</t>
   </si>
 </sst>
 </file>
@@ -447,18 +447,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA5B94D-C459-4446-A58C-6B64BB3B0F08}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C1" s="1">
         <v>2019</v>
@@ -475,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>1314</v>
@@ -492,7 +492,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>314</v>
@@ -509,7 +509,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>280</v>
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <v>1812</v>
@@ -543,7 +543,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>35</v>
@@ -560,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>16</v>
@@ -577,7 +577,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1">
         <v>965</v>
@@ -594,7 +594,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1">
         <v>329</v>
@@ -611,7 +611,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>145</v>
@@ -625,10 +625,10 @@
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C11" s="1">
         <v>1240</v>
@@ -642,10 +642,10 @@
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1">
         <v>367</v>
@@ -659,10 +659,10 @@
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -676,10 +676,10 @@
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2">
         <v>93.625</v>
@@ -693,10 +693,10 @@
     </row>
     <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="2">
         <v>65.0625</v>
@@ -710,10 +710,10 @@
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="2">
         <v>23.661460000000002</v>

</xml_diff>